<commit_message>
Cambio hashmap producto (pedido),  corrección exportación DATE
</commit_message>
<xml_diff>
--- a/pedidos.xlsx
+++ b/pedidos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaavi\Documents\laCartaDeNanaYRene\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F0EA9E-DA13-4F12-AA99-26D6595C4129}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2357EE7-D518-4C1E-9C92-6F6188A716F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{778E779E-9277-4041-8CE5-9873CE8EAF3E}"/>
+    <workbookView xWindow="1596" yWindow="2376" windowWidth="17280" windowHeight="8904" xr2:uid="{778E779E-9277-4041-8CE5-9873CE8EAF3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,21 +33,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
-    <t>torta</t>
-  </si>
-  <si>
-    <t>kuchen manzana</t>
-  </si>
-  <si>
-    <t>trozo queque</t>
-  </si>
-  <si>
-    <t>pie de limon</t>
-  </si>
-  <si>
-    <t>tartaleta durazno</t>
-  </si>
-  <si>
     <t>alberto hurtado</t>
   </si>
   <si>
@@ -84,9 +69,6 @@
     <t>Tipo de producto</t>
   </si>
   <si>
-    <t>Cantidad</t>
-  </si>
-  <si>
     <t>Fecha de solicitud</t>
   </si>
   <si>
@@ -124,6 +106,24 @@
   </si>
   <si>
     <t>9-38274654</t>
+  </si>
+  <si>
+    <t>Precio total</t>
+  </si>
+  <si>
+    <t>1-kuchen manzana</t>
+  </si>
+  <si>
+    <t>1-trozo queque</t>
+  </si>
+  <si>
+    <t>1-pie de limon</t>
+  </si>
+  <si>
+    <t>1-tartaleta durazno</t>
+  </si>
+  <si>
+    <t>1-torta,2-queques</t>
   </si>
 </sst>
 </file>
@@ -175,12 +175,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -499,79 +501,78 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" style="3"/>
-    <col min="3" max="3" width="17.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.21875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" style="2"/>
+    <col min="2" max="2" width="17.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.21875" style="2" customWidth="1"/>
+    <col min="7" max="8" width="11.5546875" style="2"/>
     <col min="9" max="9" width="15.33203125" style="3" customWidth="1"/>
     <col min="10" max="10" width="18.77734375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3">
-        <v>2</v>
+        <v>30</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43743</v>
       </c>
       <c r="C2" s="1">
-        <v>43743</v>
-      </c>
-      <c r="D2" s="1">
         <v>43744</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>15</v>
+      <c r="H2" s="6">
+        <v>1000</v>
       </c>
       <c r="I2" s="3">
         <v>0</v>
@@ -581,29 +582,29 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43744</v>
+      </c>
+      <c r="C3" s="1">
+        <v>43745</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1">
-        <v>43744</v>
-      </c>
-      <c r="D3" s="1">
-        <v>43745</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>11</v>
+      <c r="F3" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="H3" s="6">
+        <v>2000</v>
       </c>
       <c r="I3" s="3">
         <v>0</v>
@@ -614,28 +615,28 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3">
-        <v>3</v>
+        <v>27</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43745</v>
       </c>
       <c r="C4" s="1">
         <v>43745</v>
       </c>
-      <c r="D4" s="1">
-        <v>43745</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>12</v>
+      <c r="F4" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="H4" s="6">
+        <v>3000</v>
       </c>
       <c r="I4" s="3">
         <v>0</v>
@@ -646,28 +647,28 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43768</v>
+      </c>
+      <c r="C5" s="1">
+        <v>43769</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1">
-        <v>43768</v>
-      </c>
-      <c r="D5" s="1">
-        <v>43769</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>13</v>
+      <c r="F5" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="H5" s="6">
+        <v>4900</v>
       </c>
       <c r="I5" s="3">
         <v>0</v>
@@ -678,28 +679,28 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="1">
+        <v>43767</v>
+      </c>
+      <c r="C6" s="1">
+        <v>43799</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
-        <v>43767</v>
-      </c>
-      <c r="D6" s="1">
-        <v>43799</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>14</v>
+      <c r="F6" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="H6" s="6">
+        <v>5000</v>
       </c>
       <c r="I6" s="3">
         <v>0</v>
@@ -710,11 +711,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{8AEBDDC4-71AA-4301-A4E9-AE4ECD6D45D1}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{D052FC99-0405-489B-9273-235369325D0D}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{8EDF48AF-E6B3-4977-88A4-293C119A9F81}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{B81AEA45-2423-44AD-B647-895F7CB12FA5}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{568D2103-AB29-437B-8AD8-E149EFC4B464}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{8AEBDDC4-71AA-4301-A4E9-AE4ECD6D45D1}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{D052FC99-0405-489B-9273-235369325D0D}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{8EDF48AF-E6B3-4977-88A4-293C119A9F81}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{B81AEA45-2423-44AD-B647-895F7CB12FA5}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{568D2103-AB29-437B-8AD8-E149EFC4B464}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>

</xml_diff>